<commit_message>
Updated the shopping list with the actual costs and the pruchases from Kjell so that the team knows about the remainig budget.
</commit_message>
<xml_diff>
--- a/Documentation/Shopping List_modified_v02.xlsx
+++ b/Documentation/Shopping List_modified_v02.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26405"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14840"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="22120"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="88">
   <si>
     <t>Item</t>
   </si>
@@ -68,15 +68,6 @@
   </si>
   <si>
     <t>Kjell prices</t>
-  </si>
-  <si>
-    <t>Remote control batteries</t>
-  </si>
-  <si>
-    <t>4G sim card</t>
-  </si>
-  <si>
-    <t>Get one by our self,  we only require to refill it</t>
   </si>
   <si>
     <t>Quantity</t>
@@ -314,6 +305,33 @@
   </si>
   <si>
     <t>Received</t>
+  </si>
+  <si>
+    <t>Given to the team</t>
+  </si>
+  <si>
+    <t>tracking</t>
+  </si>
+  <si>
+    <t>Parcelforce.com, EK302047848GB</t>
+  </si>
+  <si>
+    <t>http://www.fedex.com/Tracking?action=track&amp;tracknumbers=781573340714</t>
+  </si>
+  <si>
+    <t>https://tools.usps.com/go/TrackConfirmAction_input?qtc_tLabels1=LJ860884362US</t>
+  </si>
+  <si>
+    <t>Actual cost (homw much was actually paid *)</t>
+  </si>
+  <si>
+    <t>* = difference is due to exchange rate that was different than estimated, payment fees such as Paypal fees etc</t>
+  </si>
+  <si>
+    <t>Buntband 300-pack</t>
+  </si>
+  <si>
+    <t>Remote control batteries 20-pack</t>
   </si>
 </sst>
 </file>
@@ -492,8 +510,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="65">
+  <cellStyleXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -615,7 +641,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="65">
+  <cellStyles count="73">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -648,6 +674,10 @@
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -680,6 +710,10 @@
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -950,7 +984,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -958,10 +992,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:O22"/>
+  <dimension ref="A2:S22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -973,27 +1007,27 @@
     <col min="5" max="6" width="12.33203125" style="10" customWidth="1"/>
     <col min="7" max="7" width="10" style="10" customWidth="1"/>
     <col min="8" max="9" width="14" style="10" customWidth="1"/>
-    <col min="10" max="10" width="24.5" style="10" customWidth="1"/>
-    <col min="11" max="11" width="89.6640625" style="10" customWidth="1"/>
-    <col min="12" max="12" width="12.5" style="10" customWidth="1"/>
-    <col min="13" max="16384" width="8.83203125" style="10"/>
+    <col min="10" max="11" width="24.5" style="10" customWidth="1"/>
+    <col min="12" max="12" width="89.6640625" style="10" customWidth="1"/>
+    <col min="13" max="13" width="12.5" style="10" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="10"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:19">
       <c r="B2" s="10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="10" t="s">
-        <v>27</v>
-      </c>
       <c r="G2" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
       <c r="C3" s="10">
         <v>8.3376000000000001</v>
       </c>
@@ -1004,55 +1038,69 @@
         <v>9.4665999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15" thickBot="1"/>
-    <row r="7" spans="1:15">
+    <row r="4" spans="1:19">
+      <c r="K4" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="15" thickBot="1"/>
+    <row r="7" spans="1:19">
       <c r="A7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="5" t="s">
         <v>1</v>
       </c>
       <c r="K7" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="L7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="L7" s="6" t="s">
+      <c r="M7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="M7" s="10" t="s">
-        <v>37</v>
-      </c>
       <c r="N7" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="O7" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="P7" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q7" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="S7" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="O7" s="10" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8" s="16" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B8" s="2">
         <v>1</v>
@@ -1072,7 +1120,7 @@
         <v>241.79999999999998</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H8" s="2">
         <f>$E$3</f>
@@ -1083,22 +1131,31 @@
         <f>F8*H8</f>
         <v>3110.8537199999996</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="K8" s="14">
+        <v>3122.84</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="M8" s="10" t="s">
-        <v>38</v>
+      <c r="M8" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="N8" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
+        <v>35</v>
+      </c>
+      <c r="O8" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="P8" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q8" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9" s="16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B9" s="2">
         <v>1</v>
@@ -1118,7 +1175,7 @@
         <v>154.99</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H9" s="2">
         <f>$E$3</f>
@@ -1129,17 +1186,29 @@
         <f>F9*H9</f>
         <v>1994.0083460000001</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="K9" s="14">
+        <v>2001.69</v>
+      </c>
+      <c r="L9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L9" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="M9" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
+      <c r="M9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N9" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="O9" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="P9" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q9" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1150,12 +1219,13 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="14"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="3"/>
-    </row>
-    <row r="11" spans="1:15">
+      <c r="K10" s="14"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="3"/>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B11" s="2">
         <v>2</v>
@@ -1175,7 +1245,7 @@
         <v>230.32</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H11" s="2">
         <f>$C$3</f>
@@ -1186,19 +1256,34 @@
         <f t="shared" ref="J11:J21" si="1">F11*H11</f>
         <v>1920.316032</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="K11" s="14">
+        <v>2019.89</v>
+      </c>
+      <c r="L11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="L11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="M11" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15">
+      <c r="M11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N11" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="O11" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="P11" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q11" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="S11" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12" s="16" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B12" s="2">
         <v>2</v>
@@ -1218,7 +1303,7 @@
         <v>3180</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H12" s="2">
         <v>1</v>
@@ -1228,15 +1313,27 @@
         <f t="shared" si="1"/>
         <v>3180</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="K12" s="14">
+        <v>3389.9</v>
+      </c>
+      <c r="L12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="L12" s="3"/>
-      <c r="M12" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15">
+      <c r="M12" s="3"/>
+      <c r="N12" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="O12" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="P12" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q12" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1247,12 +1344,13 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="14"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="3"/>
-    </row>
-    <row r="14" spans="1:15">
+      <c r="K13" s="14"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="3"/>
+    </row>
+    <row r="14" spans="1:19">
       <c r="A14" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B14" s="2">
         <v>2</v>
@@ -1272,7 +1370,7 @@
         <v>226.5</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H14" s="2">
         <f>$C$3</f>
@@ -1283,17 +1381,32 @@
         <f t="shared" si="1"/>
         <v>1888.4664</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="K14" s="14">
+        <v>1940.62</v>
+      </c>
+      <c r="L14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L14" s="3"/>
-      <c r="M14" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15">
+      <c r="M14" s="3"/>
+      <c r="N14" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="O14" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="P14" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q14" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="S14" s="10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
       <c r="A15" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B15" s="2">
         <v>2</v>
@@ -1313,7 +1426,7 @@
         <v>98</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H15" s="2">
         <f>$C$3</f>
@@ -1324,15 +1437,27 @@
         <f t="shared" si="1"/>
         <v>817.08479999999997</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="K15" s="14">
+        <v>839.65</v>
+      </c>
+      <c r="L15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L15" s="3"/>
-      <c r="M15" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15">
+      <c r="M15" s="3"/>
+      <c r="N15" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="O15" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="P15" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q15" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1343,12 +1468,13 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="14"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="3"/>
-    </row>
-    <row r="17" spans="1:12">
+      <c r="K16" s="14"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="3"/>
+    </row>
+    <row r="17" spans="1:19">
       <c r="A17" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B17" s="2">
         <v>2</v>
@@ -1368,7 +1494,7 @@
         <v>112.88999999999999</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H17" s="2">
         <f>$C$3</f>
@@ -1379,14 +1505,32 @@
         <f t="shared" si="1"/>
         <v>941.23166399999991</v>
       </c>
-      <c r="K17" s="2" t="s">
+      <c r="K17" s="14">
+        <v>960.16</v>
+      </c>
+      <c r="L17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L17" s="3" t="s">
+      <c r="M17" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:12">
+      <c r="N17" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="O17" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="P17" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q17" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="S17" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19">
       <c r="A18" s="11" t="s">
         <v>12</v>
       </c>
@@ -1399,10 +1543,11 @@
       <c r="H18" s="12"/>
       <c r="I18" s="12"/>
       <c r="J18" s="14"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="13"/>
-    </row>
-    <row r="19" spans="1:12">
+      <c r="K18" s="14"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="13"/>
+    </row>
+    <row r="19" spans="1:19">
       <c r="A19" s="11" t="s">
         <v>13</v>
       </c>
@@ -1410,58 +1555,60 @@
         <v>1</v>
       </c>
       <c r="C19" s="12">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E19" s="12">
         <v>0</v>
       </c>
       <c r="F19" s="2">
         <f t="shared" si="2"/>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H19" s="12">
         <v>1</v>
       </c>
       <c r="I19" s="12"/>
       <c r="J19" s="14">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="K19" s="12"/>
-      <c r="L19" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="K19" s="14">
+        <v>149</v>
+      </c>
+      <c r="L19" s="12"/>
+      <c r="M19" s="13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:19">
       <c r="A20" s="11" t="s">
-        <v>15</v>
+        <v>87</v>
       </c>
       <c r="B20" s="12">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C20" s="12">
-        <v>5</v>
+        <v>59.9</v>
       </c>
       <c r="D20" s="2">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>59.9</v>
       </c>
       <c r="E20" s="12">
         <v>0</v>
       </c>
       <c r="F20" s="2">
         <f t="shared" si="2"/>
-        <v>60</v>
+        <v>59.9</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H20" s="12">
         <v>1</v>
@@ -1469,36 +1616,39 @@
       <c r="I20" s="12"/>
       <c r="J20" s="14">
         <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-      <c r="K20" s="12"/>
-      <c r="L20" s="13" t="s">
+        <v>59.9</v>
+      </c>
+      <c r="K20" s="14">
+        <v>59.9</v>
+      </c>
+      <c r="L20" s="12"/>
+      <c r="M20" s="13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:19">
       <c r="A21" s="11" t="s">
-        <v>16</v>
+        <v>86</v>
       </c>
       <c r="B21" s="12">
         <v>1</v>
       </c>
       <c r="C21" s="12">
-        <v>300</v>
+        <v>29.9</v>
       </c>
       <c r="D21" s="2">
         <f t="shared" si="0"/>
-        <v>300</v>
+        <v>29.9</v>
       </c>
       <c r="E21" s="12">
         <v>0</v>
       </c>
       <c r="F21" s="2">
         <f t="shared" si="2"/>
-        <v>300</v>
+        <v>29.9</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H21" s="12">
         <v>1</v>
@@ -1506,14 +1656,15 @@
       <c r="I21" s="12"/>
       <c r="J21" s="14">
         <f t="shared" si="1"/>
-        <v>300</v>
-      </c>
-      <c r="K21" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="L21" s="15"/>
-    </row>
-    <row r="22" spans="1:12" ht="15" thickBot="1">
+        <v>29.9</v>
+      </c>
+      <c r="K21" s="14">
+        <v>29.9</v>
+      </c>
+      <c r="L21" s="12"/>
+      <c r="M21" s="15"/>
+    </row>
+    <row r="22" spans="1:19" ht="15" thickBot="1">
       <c r="A22" s="7" t="s">
         <v>11</v>
       </c>
@@ -1527,10 +1678,14 @@
       <c r="I22" s="8"/>
       <c r="J22" s="17">
         <f>SUM(J8:J21)</f>
-        <v>14311.960962000001</v>
-      </c>
-      <c r="K22" s="8"/>
-      <c r="L22" s="9"/>
+        <v>14090.760962</v>
+      </c>
+      <c r="K22" s="17">
+        <f>SUM(K8:K21)</f>
+        <v>14513.550000000001</v>
+      </c>
+      <c r="L22" s="8"/>
+      <c r="M22" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1559,10 +1714,10 @@
   <sheetData>
     <row r="2" spans="2:9">
       <c r="B2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="2:9">
@@ -1577,81 +1732,81 @@
     </row>
     <row r="4" spans="2:9">
       <c r="B4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="2:9">
       <c r="B5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="2:9">
       <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" t="s">
         <v>42</v>
       </c>
-      <c r="C7" t="s">
+      <c r="F7" t="s">
         <v>43</v>
-      </c>
-      <c r="D7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="8" spans="2:9">
       <c r="B8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="2:9">
       <c r="B9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" t="s">
         <v>50</v>
       </c>
-      <c r="C9" t="s">
+      <c r="F9" t="s">
         <v>51</v>
-      </c>
-      <c r="D9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E9" t="s">
-        <v>53</v>
-      </c>
-      <c r="F9" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="11" spans="2:9">
       <c r="B11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="2:9">
       <c r="B14" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="2:9">
       <c r="B15" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="2:9">
@@ -1666,55 +1821,55 @@
     </row>
     <row r="18" spans="2:9">
       <c r="B18" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C18" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="2:9">
       <c r="B19" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="2:9">
       <c r="B21" s="19" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="2:9">
       <c r="B22" s="19" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="2:9">
       <c r="B23" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="2:9">
       <c r="B24" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="2:9">
       <c r="B25" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="2:9">
       <c r="B26" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="2:9">
       <c r="B27" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="2:9" ht="16">
       <c r="B28" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="2:9">
@@ -1729,30 +1884,30 @@
     </row>
     <row r="31" spans="2:9">
       <c r="B31" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C31" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="2:2">
       <c r="B34" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="2:2">
       <c r="B35" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="2:2">
       <c r="B36" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the list after last meeting
</commit_message>
<xml_diff>
--- a/Documentation/Shopping List_modified_v02.xlsx
+++ b/Documentation/Shopping List_modified_v02.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26405"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="22120"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="13176"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Mobile Subscriptions" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="113">
   <si>
     <t>Item</t>
   </si>
@@ -333,12 +333,90 @@
   <si>
     <t>Remote control batteries 20-pack</t>
   </si>
+  <si>
+    <t>Screws Nylon M3 30mm</t>
+  </si>
+  <si>
+    <t>Nuts Nylon M3</t>
+  </si>
+  <si>
+    <t>USB2FTDI</t>
+  </si>
+  <si>
+    <t>Connector DF13-5S-1.25C</t>
+  </si>
+  <si>
+    <t>Crimped Cable DF13 Red</t>
+  </si>
+  <si>
+    <t>Crimped Cable DF13 Black</t>
+  </si>
+  <si>
+    <t>https://www.elfa.se/sv/cheese-head-screws-polyamide-m3-30-mm-bossard-group-bn-1061-m3x30mm/p/14842955?q=*&amp;filter_Category3=Skruv%2C+plugg+och+fj%C3%A4drar&amp;filter_Category4=Skruvar&amp;filter_Material=Plast&amp;filter_Material=Polyamid+6.6&amp;filter_G%C3%A4nga=M3&amp;filter_Buyable=1&amp;page=12&amp;origPageSize=50&amp;simi=99.5</t>
+  </si>
+  <si>
+    <t>https://www.elfa.se/sv/sexkantsmutter-polyamid-m3-richco-496239/p/14850012?q=*&amp;filter_Category3=Skruv%2C+plugg+och+fj%C3%A4drar&amp;filter_Category4=Muttrar&amp;filter_Material=Polyamid+6.6&amp;filter_G%C3%A4nga=M3&amp;filter_Buyable=1&amp;page=2&amp;origPageSize=50&amp;simi=99.5</t>
+  </si>
+  <si>
+    <t>https://www.elfa.se/sv/usb-kablage-usb-ttl-cmos-ftdi-ttl-232r-5v/p/17320673?q=17320673&amp;page=1&amp;origPos=1&amp;origPageSize=50&amp;simi=99.5</t>
+  </si>
+  <si>
+    <t>https://www.elfa.se/sv/kontakthus-25-mm-poltal-df13-hirose-df13-5s-25c/p/14352123?q=df13&amp;page=3&amp;origPos=4&amp;origPageSize=50&amp;simi=99.33</t>
+  </si>
+  <si>
+    <t>https://www.elfa.se/sv/faerdigcrimp-kablage-df13-roed-100-mm-stig-wahlstroem-elektronik-k120121010/p/14352220</t>
+  </si>
+  <si>
+    <t>https://www.elfa.se/sv/faerdigcrimp-kablage-df13-svart-100-mm-stig-wahlstroem-elektronik-k120121014/p/14352224</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Pick up Solna and pay by team</t>
+  </si>
+  <si>
+    <t>Connection Cables</t>
+  </si>
+  <si>
+    <t>Ultrasound Sensor Maxbotix HRLV-EZ4</t>
+  </si>
+  <si>
+    <t>RVVP 4x0.2 skärmad svart</t>
+  </si>
+  <si>
+    <t>http://www.electrokit.com/testsladdar-med-krokodilklammor-30mm-50cm-10pack.44765</t>
+  </si>
+  <si>
+    <t>http://www.electrokit.com/avstandsmatare-ultraljud-maxbotix-hrlvez4.49754</t>
+  </si>
+  <si>
+    <t>http://www.electrokit.com/rvvp-4x0-2-skarmad-svart-m.44669</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>6V battery (Varta 4R25)</t>
+  </si>
+  <si>
+    <t>Banan plugs</t>
+  </si>
+  <si>
+    <t>http://www.kjell.com/se/sortiment/el/batterier/specialbatteri-blockbatteri/varta-6-v-batteri-%284r25%29-p32144</t>
+  </si>
+  <si>
+    <t>http://www.kjell.com/se/sortiment/el/verktyg/matinstrument/matsladdar-prober-kontakter/labbkontakter-4-mm/4-mm-labbpropp-39-mm-svart-p37872</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;kr&quot;;[Red]\-#,##0.00\ &quot;kr&quot;"/>
+  </numFmts>
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -585,7 +663,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -640,80 +718,89 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="73">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -984,7 +1071,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -992,25 +1079,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:S22"/>
+  <dimension ref="A2:S38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="F13" workbookViewId="0">
+      <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="73.33203125" style="10" customWidth="1"/>
     <col min="2" max="2" width="30.33203125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" style="10" customWidth="1"/>
-    <col min="4" max="4" width="23.83203125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="12.77734375" style="10" customWidth="1"/>
+    <col min="4" max="4" width="23.77734375" style="10" customWidth="1"/>
     <col min="5" max="6" width="12.33203125" style="10" customWidth="1"/>
     <col min="7" max="7" width="10" style="10" customWidth="1"/>
     <col min="8" max="9" width="14" style="10" customWidth="1"/>
-    <col min="10" max="11" width="24.5" style="10" customWidth="1"/>
+    <col min="10" max="11" width="24.44140625" style="10" customWidth="1"/>
     <col min="12" max="12" width="89.6640625" style="10" customWidth="1"/>
-    <col min="13" max="13" width="12.5" style="10" customWidth="1"/>
-    <col min="14" max="16384" width="8.83203125" style="10"/>
+    <col min="13" max="13" width="12.44140625" style="10" customWidth="1"/>
+    <col min="14" max="16384" width="8.77734375" style="10"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:19">
@@ -1234,7 +1321,7 @@
         <v>89.99</v>
       </c>
       <c r="D11" s="2">
-        <f t="shared" ref="D11:D21" si="0">B11*C11</f>
+        <f t="shared" ref="D11:D36" si="0">B11*C11</f>
         <v>179.98</v>
       </c>
       <c r="E11" s="2">
@@ -1253,7 +1340,7 @@
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="14">
-        <f t="shared" ref="J11:J21" si="1">F11*H11</f>
+        <f t="shared" ref="J11:J36" si="1">F11*H11</f>
         <v>1920.316032</v>
       </c>
       <c r="K11" s="14">
@@ -1299,7 +1386,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="2">
-        <f t="shared" ref="F12:F21" si="2">D12+E12</f>
+        <f t="shared" ref="F12:F36" si="2">D12+E12</f>
         <v>3180</v>
       </c>
       <c r="G12" s="2" t="s">
@@ -1531,165 +1618,743 @@
       </c>
     </row>
     <row r="18" spans="1:19">
-      <c r="A18" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="14"/>
+      <c r="A18" s="1"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="K18" s="14"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="13"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="3"/>
     </row>
     <row r="19" spans="1:19">
-      <c r="A19" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="12">
+      <c r="A19" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B19" s="2">
         <v>1</v>
       </c>
-      <c r="C19" s="12">
-        <v>0</v>
+      <c r="C19" s="22">
+        <v>29</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E19" s="12">
-        <v>0</v>
+        <v>29</v>
+      </c>
+      <c r="E19" s="2">
+        <v>49</v>
       </c>
       <c r="F19" s="2">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G19" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H19" s="12">
+      <c r="H19" s="2">
         <v>1</v>
       </c>
-      <c r="I19" s="12"/>
+      <c r="I19" s="2"/>
       <c r="J19" s="14">
-        <v>149</v>
-      </c>
-      <c r="K19" s="14">
-        <v>149</v>
-      </c>
-      <c r="L19" s="12"/>
-      <c r="M19" s="13" t="s">
-        <v>14</v>
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
+      <c r="K19" s="14"/>
+      <c r="L19" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M19" s="3"/>
+      <c r="N19" s="10" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:19">
-      <c r="A20" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="B20" s="12">
+      <c r="A20" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B20" s="2">
         <v>1</v>
       </c>
-      <c r="C20" s="12">
-        <v>59.9</v>
+      <c r="C20" s="22">
+        <v>369</v>
       </c>
       <c r="D20" s="2">
         <f t="shared" si="0"/>
-        <v>59.9</v>
-      </c>
-      <c r="E20" s="12">
+        <v>369</v>
+      </c>
+      <c r="E20" s="2">
         <v>0</v>
       </c>
       <c r="F20" s="2">
         <f t="shared" si="2"/>
-        <v>59.9</v>
-      </c>
-      <c r="G20" s="12" t="s">
+        <v>369</v>
+      </c>
+      <c r="G20" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H20" s="12">
+      <c r="H20" s="2">
         <v>1</v>
       </c>
-      <c r="I20" s="12"/>
+      <c r="I20" s="2"/>
       <c r="J20" s="14">
         <f t="shared" si="1"/>
-        <v>59.9</v>
-      </c>
-      <c r="K20" s="14">
-        <v>59.9</v>
-      </c>
-      <c r="L20" s="12"/>
-      <c r="M20" s="13" t="s">
-        <v>14</v>
+        <v>369</v>
+      </c>
+      <c r="K20" s="14"/>
+      <c r="L20" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="M20" s="3"/>
+      <c r="N20" s="10" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:19">
-      <c r="A21" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="B21" s="12">
-        <v>1</v>
-      </c>
-      <c r="C21" s="12">
-        <v>29.9</v>
+      <c r="A21" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B21" s="2">
+        <v>2</v>
+      </c>
+      <c r="C21" s="22">
+        <v>9.3800000000000008</v>
       </c>
       <c r="D21" s="2">
         <f t="shared" si="0"/>
-        <v>29.9</v>
-      </c>
-      <c r="E21" s="12">
+        <v>18.760000000000002</v>
+      </c>
+      <c r="E21" s="2">
         <v>0</v>
       </c>
       <c r="F21" s="2">
         <f t="shared" si="2"/>
-        <v>29.9</v>
-      </c>
-      <c r="G21" s="12" t="s">
+        <v>18.760000000000002</v>
+      </c>
+      <c r="G21" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H21" s="12">
+      <c r="H21" s="2">
         <v>1</v>
       </c>
-      <c r="I21" s="12"/>
+      <c r="I21" s="2"/>
       <c r="J21" s="14">
         <f t="shared" si="1"/>
+        <v>18.760000000000002</v>
+      </c>
+      <c r="K21" s="14"/>
+      <c r="L21" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="M21" s="3"/>
+      <c r="N21" s="10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19">
+      <c r="A22" s="1"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="3"/>
+    </row>
+    <row r="23" spans="1:19">
+      <c r="A23" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="13"/>
+    </row>
+    <row r="24" spans="1:19">
+      <c r="A24" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="12">
+        <v>1</v>
+      </c>
+      <c r="C24" s="12">
+        <v>0</v>
+      </c>
+      <c r="D24" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E24" s="12">
+        <v>0</v>
+      </c>
+      <c r="F24" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H24" s="12">
+        <v>1</v>
+      </c>
+      <c r="I24" s="12"/>
+      <c r="J24" s="14">
+        <v>149</v>
+      </c>
+      <c r="K24" s="14">
+        <v>149</v>
+      </c>
+      <c r="L24" s="12"/>
+      <c r="M24" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19">
+      <c r="A25" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B25" s="12">
+        <v>1</v>
+      </c>
+      <c r="C25" s="12">
+        <v>59.9</v>
+      </c>
+      <c r="D25" s="2">
+        <f t="shared" si="0"/>
+        <v>59.9</v>
+      </c>
+      <c r="E25" s="12">
+        <v>0</v>
+      </c>
+      <c r="F25" s="2">
+        <f t="shared" si="2"/>
+        <v>59.9</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H25" s="12">
+        <v>1</v>
+      </c>
+      <c r="I25" s="12"/>
+      <c r="J25" s="14">
+        <f t="shared" si="1"/>
+        <v>59.9</v>
+      </c>
+      <c r="K25" s="14">
+        <v>59.9</v>
+      </c>
+      <c r="L25" s="12"/>
+      <c r="M25" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19">
+      <c r="A26" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="B26" s="12">
+        <v>1</v>
+      </c>
+      <c r="C26" s="12">
         <v>29.9</v>
       </c>
-      <c r="K21" s="14">
+      <c r="D26" s="2">
+        <f t="shared" si="0"/>
         <v>29.9</v>
       </c>
-      <c r="L21" s="12"/>
-      <c r="M21" s="15"/>
-    </row>
-    <row r="22" spans="1:19" ht="15" thickBot="1">
-      <c r="A22" s="7" t="s">
+      <c r="E26" s="12">
+        <v>0</v>
+      </c>
+      <c r="F26" s="2">
+        <f t="shared" si="2"/>
+        <v>29.9</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H26" s="12">
+        <v>1</v>
+      </c>
+      <c r="I26" s="12"/>
+      <c r="J26" s="14">
+        <f t="shared" si="1"/>
+        <v>29.9</v>
+      </c>
+      <c r="K26" s="14">
+        <v>29.9</v>
+      </c>
+      <c r="L26" s="12"/>
+      <c r="M26" s="15"/>
+    </row>
+    <row r="27" spans="1:19">
+      <c r="A27" s="11"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="14"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="20"/>
+    </row>
+    <row r="28" spans="1:19">
+      <c r="A28" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B28" s="12">
+        <v>30</v>
+      </c>
+      <c r="C28" s="12">
+        <v>1.39</v>
+      </c>
+      <c r="D28" s="2">
+        <f t="shared" si="0"/>
+        <v>41.699999999999996</v>
+      </c>
+      <c r="E28" s="12">
+        <v>0</v>
+      </c>
+      <c r="F28" s="2">
+        <f t="shared" si="2"/>
+        <v>41.699999999999996</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H28" s="12">
+        <v>1</v>
+      </c>
+      <c r="I28" s="12"/>
+      <c r="J28" s="14">
+        <f t="shared" si="1"/>
+        <v>41.699999999999996</v>
+      </c>
+      <c r="K28" s="14"/>
+      <c r="L28" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="M28" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="N28" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="O28" s="10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19">
+      <c r="A29" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B29" s="12">
+        <v>30</v>
+      </c>
+      <c r="C29" s="12">
+        <v>0.97</v>
+      </c>
+      <c r="D29" s="2">
+        <f t="shared" si="0"/>
+        <v>29.099999999999998</v>
+      </c>
+      <c r="E29" s="12">
+        <v>0</v>
+      </c>
+      <c r="F29" s="2">
+        <f t="shared" si="2"/>
+        <v>29.099999999999998</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H29" s="12">
+        <v>1</v>
+      </c>
+      <c r="I29" s="12"/>
+      <c r="J29" s="14">
+        <f t="shared" si="1"/>
+        <v>29.099999999999998</v>
+      </c>
+      <c r="K29" s="14"/>
+      <c r="L29" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="M29" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="N29" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="O29" s="10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19">
+      <c r="A30" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" s="12">
+        <v>1</v>
+      </c>
+      <c r="C30" s="12">
+        <v>236.25</v>
+      </c>
+      <c r="D30" s="2">
+        <f t="shared" si="0"/>
+        <v>236.25</v>
+      </c>
+      <c r="E30" s="12">
+        <v>0</v>
+      </c>
+      <c r="F30" s="2">
+        <f t="shared" si="2"/>
+        <v>236.25</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H30" s="12">
+        <v>1</v>
+      </c>
+      <c r="I30" s="12"/>
+      <c r="J30" s="14">
+        <f t="shared" si="1"/>
+        <v>236.25</v>
+      </c>
+      <c r="K30" s="14"/>
+      <c r="L30" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="M30" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="N30" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="O30" s="10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19">
+      <c r="A31" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B31" s="12">
+        <v>2</v>
+      </c>
+      <c r="C31" s="12">
+        <v>2.61</v>
+      </c>
+      <c r="D31" s="2">
+        <f t="shared" si="0"/>
+        <v>5.22</v>
+      </c>
+      <c r="E31" s="12">
+        <v>0</v>
+      </c>
+      <c r="F31" s="2">
+        <f t="shared" si="2"/>
+        <v>5.22</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H31" s="12">
+        <v>1</v>
+      </c>
+      <c r="I31" s="12"/>
+      <c r="J31" s="14">
+        <f t="shared" si="1"/>
+        <v>5.22</v>
+      </c>
+      <c r="K31" s="14"/>
+      <c r="L31" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="M31" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="N31" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="O31" s="10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19">
+      <c r="A32" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B32" s="12">
+        <v>3</v>
+      </c>
+      <c r="C32" s="12">
+        <v>10.92</v>
+      </c>
+      <c r="D32" s="2">
+        <f t="shared" si="0"/>
+        <v>32.76</v>
+      </c>
+      <c r="E32" s="12">
+        <v>0</v>
+      </c>
+      <c r="F32" s="2">
+        <f t="shared" si="2"/>
+        <v>32.76</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H32" s="12">
+        <v>1</v>
+      </c>
+      <c r="I32" s="12"/>
+      <c r="J32" s="14">
+        <f t="shared" si="1"/>
+        <v>32.76</v>
+      </c>
+      <c r="K32" s="14"/>
+      <c r="L32" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="M32" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="N32" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="O32" s="10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
+      <c r="A33" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B33" s="12">
+        <v>3</v>
+      </c>
+      <c r="C33" s="12">
+        <v>10.92</v>
+      </c>
+      <c r="D33" s="2">
+        <f t="shared" si="0"/>
+        <v>32.76</v>
+      </c>
+      <c r="E33" s="12">
+        <v>0</v>
+      </c>
+      <c r="F33" s="2">
+        <f t="shared" si="2"/>
+        <v>32.76</v>
+      </c>
+      <c r="G33" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H33" s="12">
+        <v>1</v>
+      </c>
+      <c r="I33" s="12"/>
+      <c r="J33" s="14">
+        <f t="shared" si="1"/>
+        <v>32.76</v>
+      </c>
+      <c r="K33" s="14"/>
+      <c r="L33" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="M33" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="N33" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="O33" s="10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
+      <c r="A34" s="11"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E34" s="12"/>
+      <c r="F34" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K34" s="14"/>
+      <c r="L34" s="12"/>
+      <c r="M34" s="20"/>
+    </row>
+    <row r="35" spans="1:15">
+      <c r="A35" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B35" s="12">
+        <v>4</v>
+      </c>
+      <c r="C35" s="21">
+        <v>50</v>
+      </c>
+      <c r="D35" s="2">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="E35" s="12">
+        <v>0</v>
+      </c>
+      <c r="F35" s="2">
+        <f t="shared" si="2"/>
+        <v>200</v>
+      </c>
+      <c r="G35" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H35" s="12">
+        <v>1</v>
+      </c>
+      <c r="I35" s="12"/>
+      <c r="J35" s="14">
+        <f t="shared" si="1"/>
+        <v>200</v>
+      </c>
+      <c r="K35" s="14"/>
+      <c r="L35" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="M35" s="20"/>
+    </row>
+    <row r="36" spans="1:15">
+      <c r="A36" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="B36" s="12">
+        <v>2</v>
+      </c>
+      <c r="C36" s="21">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="D36" s="2">
+        <f t="shared" si="0"/>
+        <v>35.799999999999997</v>
+      </c>
+      <c r="E36" s="12">
+        <v>0</v>
+      </c>
+      <c r="F36" s="2">
+        <f t="shared" si="2"/>
+        <v>35.799999999999997</v>
+      </c>
+      <c r="G36" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H36" s="12">
+        <v>1</v>
+      </c>
+      <c r="I36" s="12"/>
+      <c r="J36" s="14">
+        <f t="shared" si="1"/>
+        <v>35.799999999999997</v>
+      </c>
+      <c r="K36" s="14"/>
+      <c r="L36" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="M36" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="N36" s="10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
+      <c r="A37" s="11"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="14"/>
+      <c r="K37" s="14"/>
+      <c r="L37" s="12"/>
+      <c r="M37" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="N37" s="10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="15" thickBot="1">
+      <c r="A38" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="17">
-        <f>SUM(J8:J21)</f>
-        <v>14090.760962</v>
-      </c>
-      <c r="K22" s="17">
-        <f>SUM(K8:K21)</f>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="17">
+        <f>SUM(J8:J36)</f>
+        <v>15170.110962000001</v>
+      </c>
+      <c r="K38" s="17">
+        <f>SUM(K8:K36)</f>
         <v>14513.550000000001</v>
       </c>
-      <c r="L22" s="8"/>
-      <c r="M22" s="9"/>
+      <c r="L38" s="8"/>
+      <c r="M38" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1706,7 +2371,7 @@
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="24.33203125" customWidth="1"/>
     <col min="3" max="3" width="6" customWidth="1"/>
@@ -1867,7 +2532,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="2:9" ht="16">
+    <row r="28" spans="2:9" ht="16.2">
       <c r="B28" t="s">
         <v>68</v>
       </c>

</xml_diff>

<commit_message>
Revert "Updated the list after last meeting"
This reverts commit 3254081db75cd6923d555d48abc6a98fd921d763.
</commit_message>
<xml_diff>
--- a/Documentation/Shopping List_modified_v02.xlsx
+++ b/Documentation/Shopping List_modified_v02.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26405"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="13176"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="22120"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Mobile Subscriptions" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="88">
   <si>
     <t>Item</t>
   </si>
@@ -333,90 +333,12 @@
   <si>
     <t>Remote control batteries 20-pack</t>
   </si>
-  <si>
-    <t>Screws Nylon M3 30mm</t>
-  </si>
-  <si>
-    <t>Nuts Nylon M3</t>
-  </si>
-  <si>
-    <t>USB2FTDI</t>
-  </si>
-  <si>
-    <t>Connector DF13-5S-1.25C</t>
-  </si>
-  <si>
-    <t>Crimped Cable DF13 Red</t>
-  </si>
-  <si>
-    <t>Crimped Cable DF13 Black</t>
-  </si>
-  <si>
-    <t>https://www.elfa.se/sv/cheese-head-screws-polyamide-m3-30-mm-bossard-group-bn-1061-m3x30mm/p/14842955?q=*&amp;filter_Category3=Skruv%2C+plugg+och+fj%C3%A4drar&amp;filter_Category4=Skruvar&amp;filter_Material=Plast&amp;filter_Material=Polyamid+6.6&amp;filter_G%C3%A4nga=M3&amp;filter_Buyable=1&amp;page=12&amp;origPageSize=50&amp;simi=99.5</t>
-  </si>
-  <si>
-    <t>https://www.elfa.se/sv/sexkantsmutter-polyamid-m3-richco-496239/p/14850012?q=*&amp;filter_Category3=Skruv%2C+plugg+och+fj%C3%A4drar&amp;filter_Category4=Muttrar&amp;filter_Material=Polyamid+6.6&amp;filter_G%C3%A4nga=M3&amp;filter_Buyable=1&amp;page=2&amp;origPageSize=50&amp;simi=99.5</t>
-  </si>
-  <si>
-    <t>https://www.elfa.se/sv/usb-kablage-usb-ttl-cmos-ftdi-ttl-232r-5v/p/17320673?q=17320673&amp;page=1&amp;origPos=1&amp;origPageSize=50&amp;simi=99.5</t>
-  </si>
-  <si>
-    <t>https://www.elfa.se/sv/kontakthus-25-mm-poltal-df13-hirose-df13-5s-25c/p/14352123?q=df13&amp;page=3&amp;origPos=4&amp;origPageSize=50&amp;simi=99.33</t>
-  </si>
-  <si>
-    <t>https://www.elfa.se/sv/faerdigcrimp-kablage-df13-roed-100-mm-stig-wahlstroem-elektronik-k120121010/p/14352220</t>
-  </si>
-  <si>
-    <t>https://www.elfa.se/sv/faerdigcrimp-kablage-df13-svart-100-mm-stig-wahlstroem-elektronik-k120121014/p/14352224</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>Pick up Solna and pay by team</t>
-  </si>
-  <si>
-    <t>Connection Cables</t>
-  </si>
-  <si>
-    <t>Ultrasound Sensor Maxbotix HRLV-EZ4</t>
-  </si>
-  <si>
-    <t>RVVP 4x0.2 skärmad svart</t>
-  </si>
-  <si>
-    <t>http://www.electrokit.com/testsladdar-med-krokodilklammor-30mm-50cm-10pack.44765</t>
-  </si>
-  <si>
-    <t>http://www.electrokit.com/avstandsmatare-ultraljud-maxbotix-hrlvez4.49754</t>
-  </si>
-  <si>
-    <t>http://www.electrokit.com/rvvp-4x0-2-skarmad-svart-m.44669</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>6V battery (Varta 4R25)</t>
-  </si>
-  <si>
-    <t>Banan plugs</t>
-  </si>
-  <si>
-    <t>http://www.kjell.com/se/sortiment/el/batterier/specialbatteri-blockbatteri/varta-6-v-batteri-%284r25%29-p32144</t>
-  </si>
-  <si>
-    <t>http://www.kjell.com/se/sortiment/el/verktyg/matinstrument/matsladdar-prober-kontakter/labbkontakter-4-mm/4-mm-labbpropp-39-mm-svart-p37872</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;kr&quot;;[Red]\-#,##0.00\ &quot;kr&quot;"/>
-  </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -663,7 +585,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -718,89 +640,80 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="73">
-    <cellStyle name="Följd hyperlänk" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlänk" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1071,7 +984,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1079,25 +992,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:S38"/>
+  <dimension ref="A2:S22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F13" workbookViewId="0">
-      <selection activeCell="J40" sqref="J40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="73.33203125" style="10" customWidth="1"/>
     <col min="2" max="2" width="30.33203125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="12.77734375" style="10" customWidth="1"/>
-    <col min="4" max="4" width="23.77734375" style="10" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" style="10" customWidth="1"/>
+    <col min="4" max="4" width="23.83203125" style="10" customWidth="1"/>
     <col min="5" max="6" width="12.33203125" style="10" customWidth="1"/>
     <col min="7" max="7" width="10" style="10" customWidth="1"/>
     <col min="8" max="9" width="14" style="10" customWidth="1"/>
-    <col min="10" max="11" width="24.44140625" style="10" customWidth="1"/>
+    <col min="10" max="11" width="24.5" style="10" customWidth="1"/>
     <col min="12" max="12" width="89.6640625" style="10" customWidth="1"/>
-    <col min="13" max="13" width="12.44140625" style="10" customWidth="1"/>
-    <col min="14" max="16384" width="8.77734375" style="10"/>
+    <col min="13" max="13" width="12.5" style="10" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="10"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:19">
@@ -1321,7 +1234,7 @@
         <v>89.99</v>
       </c>
       <c r="D11" s="2">
-        <f t="shared" ref="D11:D36" si="0">B11*C11</f>
+        <f t="shared" ref="D11:D21" si="0">B11*C11</f>
         <v>179.98</v>
       </c>
       <c r="E11" s="2">
@@ -1340,7 +1253,7 @@
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="14">
-        <f t="shared" ref="J11:J36" si="1">F11*H11</f>
+        <f t="shared" ref="J11:J21" si="1">F11*H11</f>
         <v>1920.316032</v>
       </c>
       <c r="K11" s="14">
@@ -1386,7 +1299,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="2">
-        <f t="shared" ref="F12:F36" si="2">D12+E12</f>
+        <f t="shared" ref="F12:F21" si="2">D12+E12</f>
         <v>3180</v>
       </c>
       <c r="G12" s="2" t="s">
@@ -1618,743 +1531,165 @@
       </c>
     </row>
     <row r="18" spans="1:19">
-      <c r="A18" s="1"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2">
+      <c r="A18" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="13"/>
+    </row>
+    <row r="19" spans="1:19">
+      <c r="A19" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="12">
+        <v>1</v>
+      </c>
+      <c r="C19" s="12">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2">
+      <c r="E19" s="12">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K18" s="14"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="3"/>
-    </row>
-    <row r="19" spans="1:19">
-      <c r="A19" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B19" s="2">
+      <c r="G19" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" s="12">
         <v>1</v>
       </c>
-      <c r="C19" s="22">
-        <v>29</v>
-      </c>
-      <c r="D19" s="2">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="E19" s="2">
-        <v>49</v>
-      </c>
-      <c r="F19" s="2">
-        <f t="shared" si="2"/>
-        <v>78</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H19" s="2">
+      <c r="I19" s="12"/>
+      <c r="J19" s="14">
+        <v>149</v>
+      </c>
+      <c r="K19" s="14">
+        <v>149</v>
+      </c>
+      <c r="L19" s="12"/>
+      <c r="M19" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19">
+      <c r="A20" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" s="12">
         <v>1</v>
       </c>
-      <c r="I19" s="2"/>
-      <c r="J19" s="14">
-        <f t="shared" si="1"/>
-        <v>78</v>
-      </c>
-      <c r="K19" s="14"/>
-      <c r="L19" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="M19" s="3"/>
-      <c r="N19" s="10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19">
-      <c r="A20" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B20" s="2">
-        <v>1</v>
-      </c>
-      <c r="C20" s="22">
-        <v>369</v>
+      <c r="C20" s="12">
+        <v>59.9</v>
       </c>
       <c r="D20" s="2">
         <f t="shared" si="0"/>
-        <v>369</v>
-      </c>
-      <c r="E20" s="2">
+        <v>59.9</v>
+      </c>
+      <c r="E20" s="12">
         <v>0</v>
       </c>
       <c r="F20" s="2">
         <f t="shared" si="2"/>
-        <v>369</v>
-      </c>
-      <c r="G20" s="2" t="s">
+        <v>59.9</v>
+      </c>
+      <c r="G20" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H20" s="12">
         <v>1</v>
       </c>
-      <c r="I20" s="2"/>
+      <c r="I20" s="12"/>
       <c r="J20" s="14">
         <f t="shared" si="1"/>
-        <v>369</v>
-      </c>
-      <c r="K20" s="14"/>
-      <c r="L20" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="M20" s="3"/>
-      <c r="N20" s="10" t="s">
-        <v>108</v>
+        <v>59.9</v>
+      </c>
+      <c r="K20" s="14">
+        <v>59.9</v>
+      </c>
+      <c r="L20" s="12"/>
+      <c r="M20" s="13" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:19">
-      <c r="A21" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B21" s="2">
-        <v>2</v>
-      </c>
-      <c r="C21" s="22">
-        <v>9.3800000000000008</v>
+      <c r="A21" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" s="12">
+        <v>1</v>
+      </c>
+      <c r="C21" s="12">
+        <v>29.9</v>
       </c>
       <c r="D21" s="2">
         <f t="shared" si="0"/>
-        <v>18.760000000000002</v>
-      </c>
-      <c r="E21" s="2">
+        <v>29.9</v>
+      </c>
+      <c r="E21" s="12">
         <v>0</v>
       </c>
       <c r="F21" s="2">
         <f t="shared" si="2"/>
-        <v>18.760000000000002</v>
-      </c>
-      <c r="G21" s="2" t="s">
+        <v>29.9</v>
+      </c>
+      <c r="G21" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="H21" s="2">
+      <c r="H21" s="12">
         <v>1</v>
       </c>
-      <c r="I21" s="2"/>
+      <c r="I21" s="12"/>
       <c r="J21" s="14">
         <f t="shared" si="1"/>
-        <v>18.760000000000002</v>
-      </c>
-      <c r="K21" s="14"/>
-      <c r="L21" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="M21" s="3"/>
-      <c r="N21" s="10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19">
-      <c r="A22" s="1"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="3"/>
-    </row>
-    <row r="23" spans="1:19">
-      <c r="A23" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="12"/>
-      <c r="M23" s="13"/>
-    </row>
-    <row r="24" spans="1:19">
-      <c r="A24" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="12">
-        <v>1</v>
-      </c>
-      <c r="C24" s="12">
-        <v>0</v>
-      </c>
-      <c r="D24" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E24" s="12">
-        <v>0</v>
-      </c>
-      <c r="F24" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G24" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H24" s="12">
-        <v>1</v>
-      </c>
-      <c r="I24" s="12"/>
-      <c r="J24" s="14">
-        <v>149</v>
-      </c>
-      <c r="K24" s="14">
-        <v>149</v>
-      </c>
-      <c r="L24" s="12"/>
-      <c r="M24" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19">
-      <c r="A25" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="B25" s="12">
-        <v>1</v>
-      </c>
-      <c r="C25" s="12">
-        <v>59.9</v>
-      </c>
-      <c r="D25" s="2">
-        <f t="shared" si="0"/>
-        <v>59.9</v>
-      </c>
-      <c r="E25" s="12">
-        <v>0</v>
-      </c>
-      <c r="F25" s="2">
-        <f t="shared" si="2"/>
-        <v>59.9</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H25" s="12">
-        <v>1</v>
-      </c>
-      <c r="I25" s="12"/>
-      <c r="J25" s="14">
-        <f t="shared" si="1"/>
-        <v>59.9</v>
-      </c>
-      <c r="K25" s="14">
-        <v>59.9</v>
-      </c>
-      <c r="L25" s="12"/>
-      <c r="M25" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19">
-      <c r="A26" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="B26" s="12">
-        <v>1</v>
-      </c>
-      <c r="C26" s="12">
         <v>29.9</v>
       </c>
-      <c r="D26" s="2">
-        <f t="shared" si="0"/>
+      <c r="K21" s="14">
         <v>29.9</v>
       </c>
-      <c r="E26" s="12">
-        <v>0</v>
-      </c>
-      <c r="F26" s="2">
-        <f t="shared" si="2"/>
-        <v>29.9</v>
-      </c>
-      <c r="G26" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H26" s="12">
-        <v>1</v>
-      </c>
-      <c r="I26" s="12"/>
-      <c r="J26" s="14">
-        <f t="shared" si="1"/>
-        <v>29.9</v>
-      </c>
-      <c r="K26" s="14">
-        <v>29.9</v>
-      </c>
-      <c r="L26" s="12"/>
-      <c r="M26" s="15"/>
-    </row>
-    <row r="27" spans="1:19">
-      <c r="A27" s="11"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="12"/>
-      <c r="M27" s="20"/>
-    </row>
-    <row r="28" spans="1:19">
-      <c r="A28" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="B28" s="12">
-        <v>30</v>
-      </c>
-      <c r="C28" s="12">
-        <v>1.39</v>
-      </c>
-      <c r="D28" s="2">
-        <f t="shared" si="0"/>
-        <v>41.699999999999996</v>
-      </c>
-      <c r="E28" s="12">
-        <v>0</v>
-      </c>
-      <c r="F28" s="2">
-        <f t="shared" si="2"/>
-        <v>41.699999999999996</v>
-      </c>
-      <c r="G28" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H28" s="12">
-        <v>1</v>
-      </c>
-      <c r="I28" s="12"/>
-      <c r="J28" s="14">
-        <f t="shared" si="1"/>
-        <v>41.699999999999996</v>
-      </c>
-      <c r="K28" s="14"/>
-      <c r="L28" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="M28" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="N28" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="O28" s="10" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19">
-      <c r="A29" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="B29" s="12">
-        <v>30</v>
-      </c>
-      <c r="C29" s="12">
-        <v>0.97</v>
-      </c>
-      <c r="D29" s="2">
-        <f t="shared" si="0"/>
-        <v>29.099999999999998</v>
-      </c>
-      <c r="E29" s="12">
-        <v>0</v>
-      </c>
-      <c r="F29" s="2">
-        <f t="shared" si="2"/>
-        <v>29.099999999999998</v>
-      </c>
-      <c r="G29" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H29" s="12">
-        <v>1</v>
-      </c>
-      <c r="I29" s="12"/>
-      <c r="J29" s="14">
-        <f t="shared" si="1"/>
-        <v>29.099999999999998</v>
-      </c>
-      <c r="K29" s="14"/>
-      <c r="L29" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="M29" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="N29" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="O29" s="10" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19">
-      <c r="A30" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="B30" s="12">
-        <v>1</v>
-      </c>
-      <c r="C30" s="12">
-        <v>236.25</v>
-      </c>
-      <c r="D30" s="2">
-        <f t="shared" si="0"/>
-        <v>236.25</v>
-      </c>
-      <c r="E30" s="12">
-        <v>0</v>
-      </c>
-      <c r="F30" s="2">
-        <f t="shared" si="2"/>
-        <v>236.25</v>
-      </c>
-      <c r="G30" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H30" s="12">
-        <v>1</v>
-      </c>
-      <c r="I30" s="12"/>
-      <c r="J30" s="14">
-        <f t="shared" si="1"/>
-        <v>236.25</v>
-      </c>
-      <c r="K30" s="14"/>
-      <c r="L30" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="M30" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="N30" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="O30" s="10" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19">
-      <c r="A31" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="B31" s="12">
-        <v>2</v>
-      </c>
-      <c r="C31" s="12">
-        <v>2.61</v>
-      </c>
-      <c r="D31" s="2">
-        <f t="shared" si="0"/>
-        <v>5.22</v>
-      </c>
-      <c r="E31" s="12">
-        <v>0</v>
-      </c>
-      <c r="F31" s="2">
-        <f t="shared" si="2"/>
-        <v>5.22</v>
-      </c>
-      <c r="G31" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H31" s="12">
-        <v>1</v>
-      </c>
-      <c r="I31" s="12"/>
-      <c r="J31" s="14">
-        <f t="shared" si="1"/>
-        <v>5.22</v>
-      </c>
-      <c r="K31" s="14"/>
-      <c r="L31" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="M31" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="N31" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="O31" s="10" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19">
-      <c r="A32" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="B32" s="12">
-        <v>3</v>
-      </c>
-      <c r="C32" s="12">
-        <v>10.92</v>
-      </c>
-      <c r="D32" s="2">
-        <f t="shared" si="0"/>
-        <v>32.76</v>
-      </c>
-      <c r="E32" s="12">
-        <v>0</v>
-      </c>
-      <c r="F32" s="2">
-        <f t="shared" si="2"/>
-        <v>32.76</v>
-      </c>
-      <c r="G32" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H32" s="12">
-        <v>1</v>
-      </c>
-      <c r="I32" s="12"/>
-      <c r="J32" s="14">
-        <f t="shared" si="1"/>
-        <v>32.76</v>
-      </c>
-      <c r="K32" s="14"/>
-      <c r="L32" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="M32" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="N32" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="O32" s="10" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15">
-      <c r="A33" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="B33" s="12">
-        <v>3</v>
-      </c>
-      <c r="C33" s="12">
-        <v>10.92</v>
-      </c>
-      <c r="D33" s="2">
-        <f t="shared" si="0"/>
-        <v>32.76</v>
-      </c>
-      <c r="E33" s="12">
-        <v>0</v>
-      </c>
-      <c r="F33" s="2">
-        <f t="shared" si="2"/>
-        <v>32.76</v>
-      </c>
-      <c r="G33" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H33" s="12">
-        <v>1</v>
-      </c>
-      <c r="I33" s="12"/>
-      <c r="J33" s="14">
-        <f t="shared" si="1"/>
-        <v>32.76</v>
-      </c>
-      <c r="K33" s="14"/>
-      <c r="L33" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="M33" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="N33" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="O33" s="10" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15">
-      <c r="A34" s="11"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E34" s="12"/>
-      <c r="F34" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
-      <c r="I34" s="12"/>
-      <c r="J34" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K34" s="14"/>
-      <c r="L34" s="12"/>
-      <c r="M34" s="20"/>
-    </row>
-    <row r="35" spans="1:15">
-      <c r="A35" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="B35" s="12">
-        <v>4</v>
-      </c>
-      <c r="C35" s="21">
-        <v>50</v>
-      </c>
-      <c r="D35" s="2">
-        <f t="shared" si="0"/>
-        <v>200</v>
-      </c>
-      <c r="E35" s="12">
-        <v>0</v>
-      </c>
-      <c r="F35" s="2">
-        <f t="shared" si="2"/>
-        <v>200</v>
-      </c>
-      <c r="G35" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H35" s="12">
-        <v>1</v>
-      </c>
-      <c r="I35" s="12"/>
-      <c r="J35" s="14">
-        <f t="shared" si="1"/>
-        <v>200</v>
-      </c>
-      <c r="K35" s="14"/>
-      <c r="L35" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="M35" s="20"/>
-    </row>
-    <row r="36" spans="1:15">
-      <c r="A36" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="B36" s="12">
-        <v>2</v>
-      </c>
-      <c r="C36" s="21">
-        <v>17.899999999999999</v>
-      </c>
-      <c r="D36" s="2">
-        <f t="shared" si="0"/>
-        <v>35.799999999999997</v>
-      </c>
-      <c r="E36" s="12">
-        <v>0</v>
-      </c>
-      <c r="F36" s="2">
-        <f t="shared" si="2"/>
-        <v>35.799999999999997</v>
-      </c>
-      <c r="G36" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H36" s="12">
-        <v>1</v>
-      </c>
-      <c r="I36" s="12"/>
-      <c r="J36" s="14">
-        <f t="shared" si="1"/>
-        <v>35.799999999999997</v>
-      </c>
-      <c r="K36" s="14"/>
-      <c r="L36" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="M36" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="N36" s="10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15">
-      <c r="A37" s="11"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="12"/>
-      <c r="H37" s="12"/>
-      <c r="I37" s="12"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="14"/>
-      <c r="L37" s="12"/>
-      <c r="M37" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="N37" s="10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" ht="15" thickBot="1">
-      <c r="A38" s="7" t="s">
+      <c r="L21" s="12"/>
+      <c r="M21" s="15"/>
+    </row>
+    <row r="22" spans="1:19" ht="15" thickBot="1">
+      <c r="A22" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="17">
-        <f>SUM(J8:J36)</f>
-        <v>15170.110962000001</v>
-      </c>
-      <c r="K38" s="17">
-        <f>SUM(K8:K36)</f>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="17">
+        <f>SUM(J8:J21)</f>
+        <v>14090.760962</v>
+      </c>
+      <c r="K22" s="17">
+        <f>SUM(K8:K21)</f>
         <v>14513.550000000001</v>
       </c>
-      <c r="L38" s="8"/>
-      <c r="M38" s="9"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2371,7 +1706,7 @@
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="24.33203125" customWidth="1"/>
     <col min="3" max="3" width="6" customWidth="1"/>
@@ -2532,7 +1867,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="2:9" ht="16.2">
+    <row r="28" spans="2:9" ht="16">
       <c r="B28" t="s">
         <v>68</v>
       </c>

</xml_diff>